<commit_message>
task planning, planning of iteration 1
</commit_message>
<xml_diff>
--- a/prjplanning/projektplanung.xlsx
+++ b/prjplanning/projektplanung.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
   <si>
     <t xml:space="preserve"> Tag</t>
   </si>
@@ -56,9 +56,6 @@
     <t>#</t>
   </si>
   <si>
-    <t>Rest-aufwand</t>
-  </si>
-  <si>
     <t>David Elsener</t>
   </si>
   <si>
@@ -149,22 +146,88 @@
     <t>Task</t>
   </si>
   <si>
-    <t xml:space="preserve">Total </t>
-  </si>
-  <si>
-    <t>Verfügbare Zeit</t>
-  </si>
-  <si>
-    <t>Aufgewendete Zeit RK</t>
-  </si>
-  <si>
-    <t>Aufgewendete Zeit DEL</t>
-  </si>
-  <si>
-    <t>Streuli Baby hüten</t>
-  </si>
-  <si>
     <t>David</t>
+  </si>
+  <si>
+    <t>(4h pro Person)</t>
+  </si>
+  <si>
+    <t>Theorie: Aufarbeitung Thematik "Differential Gleichungen"</t>
+  </si>
+  <si>
+    <t>Theorie: Einarbeitung in Thematik "Dynamische Systeme"</t>
+  </si>
+  <si>
+    <t>Infrastruktur (Git Repo, ..)/Java-Projekt aufsetzen</t>
+  </si>
+  <si>
+    <t>Schätzung (h)</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Konzeptionell: Spezifizierung eines konkreten dynamischen Systems</t>
+  </si>
+  <si>
+    <t>(3h pro Person)</t>
+  </si>
+  <si>
+    <t>Dokumentation: 0.5-1 Seite Projektbeschreibung (inkl. des DS)</t>
+  </si>
+  <si>
+    <t>Konzeptionell: GUI Mockups (Anzeige der Grafen)</t>
+  </si>
+  <si>
+    <t>Konzeptionell: Planung der Software-Architektur für generisches Programm zur Einspeisung von dynamischen Systemen</t>
+  </si>
+  <si>
+    <t>Evaluation einer Library für die Generierung der Grafen</t>
+  </si>
+  <si>
+    <t>Implementierung der Logik zur Lösung von Differential Gleichungen</t>
+  </si>
+  <si>
+    <t>Implementierung des Basisprogramms (ohne GUI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basis-GUI (Mainframe, Menu, etc.) implementieren </t>
+  </si>
+  <si>
+    <t>Dokumentation nachführen - Teil 1</t>
+  </si>
+  <si>
+    <t>(2h pro Person)</t>
+  </si>
+  <si>
+    <t>Einbinung der Grafen-Library und Implementierung von geeigneten Schnittstellen zum Zeichnen der Grafen des dynamischen Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUI und Backend zusammenführen </t>
+  </si>
+  <si>
+    <t>Einspeisung des konkreten dynamischen Systems, erster Testlauf</t>
+  </si>
+  <si>
+    <t>Dokumentation nachführen - Teil 2</t>
+  </si>
+  <si>
+    <t>(1.5h pro Person)</t>
+  </si>
+  <si>
+    <t>Präsentation vorbereiten</t>
+  </si>
+  <si>
+    <t>Puffer / Weitere dynamische Systeme einspeisen</t>
+  </si>
+  <si>
+    <t>Aufwand total</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Restaufwand</t>
   </si>
 </sst>
 </file>
@@ -270,32 +333,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <strike/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <i/>
       <sz val="18"/>
       <color theme="1" tint="0.249977111117893"/>
@@ -309,8 +346,31 @@
       <name val="Candara"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,8 +413,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -532,22 +604,88 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
       </top>
-      <bottom style="double">
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </bottom>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -641,16 +779,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -667,26 +802,87 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,6 +892,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FFCC"/>
       <color rgb="FF5F5F5F"/>
       <color rgb="FFFFCC00"/>
       <color rgb="FFFF5050"/>
@@ -868,70 +1065,70 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>12</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1020,67 +1217,67 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.1</c:v>
+                  <c:v>38.950000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.200000000000003</c:v>
+                  <c:v>36.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.300000000000004</c:v>
+                  <c:v>34.850000000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.400000000000006</c:v>
+                  <c:v>32.800000000000011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28.500000000000007</c:v>
+                  <c:v>30.750000000000011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.600000000000009</c:v>
+                  <c:v>28.70000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.70000000000001</c:v>
+                  <c:v>26.650000000000009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.800000000000011</c:v>
+                  <c:v>24.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.900000000000013</c:v>
+                  <c:v>22.550000000000008</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.000000000000014</c:v>
+                  <c:v>20.500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.100000000000016</c:v>
+                  <c:v>18.450000000000006</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15.200000000000015</c:v>
+                  <c:v>16.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.300000000000015</c:v>
+                  <c:v>14.350000000000005</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.400000000000015</c:v>
+                  <c:v>12.300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.5000000000000142</c:v>
+                  <c:v>10.250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.6000000000000139</c:v>
+                  <c:v>8.2000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.7000000000000135</c:v>
+                  <c:v>6.150000000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.8000000000000136</c:v>
+                  <c:v>4.1000000000000032</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.9000000000000137</c:v>
+                  <c:v>2.0500000000000034</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.3766765505351941E-14</c:v>
+                  <c:v>3.5527136788005009E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1097,11 +1294,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70179456"/>
-        <c:axId val="70197632"/>
+        <c:axId val="85031936"/>
+        <c:axId val="85041920"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="70179456"/>
+        <c:axId val="85031936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1121,7 +1318,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70197632"/>
+        <c:crossAx val="85041920"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="0"/>
@@ -1132,7 +1329,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="70197632"/>
+        <c:axId val="85041920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1164,7 +1361,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70179456"/>
+        <c:crossAx val="85031936"/>
         <c:crossesAt val="41221"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -1889,21 +2086,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M11"/>
+  <dimension ref="B1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="1.140625" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="52.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="51" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" style="5" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" style="24" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" customWidth="1"/>
@@ -1915,7 +2112,7 @@
   <sheetData>
     <row r="1" spans="2:13" s="23" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B1" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
@@ -1928,7 +2125,7 @@
     </row>
     <row r="2" spans="2:13" s="23" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B2" s="43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
@@ -1957,50 +2154,58 @@
     </row>
     <row r="5" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="24"/>
+    </row>
+    <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="24"/>
-    </row>
-    <row r="7" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="37" t="s">
+      <c r="E7" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="38" t="s">
+      <c r="G7" s="67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="72">
+        <v>1</v>
+      </c>
+      <c r="C8" s="73" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="44">
-        <v>1</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>28</v>
       </c>
       <c r="D8" s="27">
         <v>18</v>
       </c>
       <c r="E8" s="27">
-        <v>20</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="44">
+        <v>23</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="68">
+        <f>SUM(D8:E8)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="74">
         <v>2</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>29</v>
+      <c r="C9" s="75" t="s">
+        <v>28</v>
       </c>
       <c r="D9" s="27">
         <v>5</v>
@@ -2008,36 +2213,365 @@
       <c r="E9" s="27">
         <v>15</v>
       </c>
-      <c r="F9" s="46" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="68">
+        <f t="shared" ref="G9:G11" si="0">SUM(D9:E9)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="44">
         <v>3</v>
       </c>
       <c r="C10" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="48">
         <v>30</v>
       </c>
-      <c r="D10" s="49">
-        <v>30</v>
-      </c>
-      <c r="E10" s="49">
-        <v>25</v>
-      </c>
-      <c r="F10" s="27"/>
-    </row>
-    <row r="11" spans="2:13" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="47">
+      <c r="E10" s="48">
+        <v>22</v>
+      </c>
+      <c r="F10" s="57"/>
+      <c r="G10" s="68">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="46">
         <f>SUM(D8:D10)</f>
         <v>53</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="47">
         <f>SUM(E8:E10)</f>
         <v>60</v>
       </c>
+      <c r="G11" s="68">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="44">
+        <v>1</v>
+      </c>
+      <c r="C16" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="58">
+        <v>8</v>
+      </c>
+      <c r="G16" s="59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="44">
+        <v>2</v>
+      </c>
+      <c r="C17" s="76" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="58">
+        <v>8</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="44">
+        <v>3</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="24"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="44">
+        <v>4</v>
+      </c>
+      <c r="C19" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="58">
+        <v>6</v>
+      </c>
+      <c r="G19" s="62" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="44">
+        <v>5</v>
+      </c>
+      <c r="C20" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="58">
+        <v>3</v>
+      </c>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="44">
+        <v>5</v>
+      </c>
+      <c r="C21" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="58">
+        <v>2</v>
+      </c>
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" spans="2:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="44">
+        <v>6</v>
+      </c>
+      <c r="C22" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="58">
+        <v>2</v>
+      </c>
+      <c r="G22" s="24"/>
+    </row>
+    <row r="23" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="44">
+        <v>7</v>
+      </c>
+      <c r="C23" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="58">
+        <v>20</v>
+      </c>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="44">
+        <v>7</v>
+      </c>
+      <c r="C24" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="58">
+        <v>10</v>
+      </c>
+      <c r="G24" s="24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+    </row>
+    <row r="25" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="44">
+        <v>8</v>
+      </c>
+      <c r="C25" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="58">
+        <v>2</v>
+      </c>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="44">
+        <v>9</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="58">
+        <v>10</v>
+      </c>
+      <c r="G26" s="24"/>
+    </row>
+    <row r="27" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="44">
+        <v>10</v>
+      </c>
+      <c r="C27" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="58">
+        <v>4</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="44">
+        <v>11</v>
+      </c>
+      <c r="C28" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="58">
+        <v>10</v>
+      </c>
+      <c r="G28" s="24"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="44">
+        <v>12</v>
+      </c>
+      <c r="C29" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="58">
+        <v>4</v>
+      </c>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="44">
+        <v>13</v>
+      </c>
+      <c r="C30" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="58">
+        <v>5</v>
+      </c>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="44">
+        <v>14</v>
+      </c>
+      <c r="C31" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="58">
+        <v>3</v>
+      </c>
+      <c r="G31" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="44">
+        <v>15</v>
+      </c>
+      <c r="C32" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="58">
+        <v>6</v>
+      </c>
+      <c r="G32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="44">
+        <v>16</v>
+      </c>
+      <c r="C33" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="58">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E35" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="63">
+        <f>SUM(F16:F33)</f>
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C21:E21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2045,10 +2579,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,32 +2593,30 @@
     <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="24" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" customWidth="1"/>
-    <col min="12" max="13" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="24" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="23" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" s="23" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="20"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="I1" s="22"/>
       <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-    </row>
-    <row r="2" spans="1:12" s="23" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:11" s="23" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A2" s="19"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -2092,11 +2624,10 @@
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
       <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-    </row>
-    <row r="3" spans="1:12" s="23" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="3" spans="1:11" s="23" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -2104,36 +2635,35 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
       <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E4" s="24"/>
       <c r="G4"/>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:12" s="25" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" s="25" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="30" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="30" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>9</v>
-      </c>
       <c r="B6" s="27">
+        <f>SUMIF(E15:E26,"Roger",D15:D26)</f>
         <v>18</v>
       </c>
       <c r="C6" s="28">
-        <f>B6-SUM(E15:E23)</f>
+        <f>B6-SUMIF(E14:E25,"Roger",F14:F25)</f>
         <v>18</v>
       </c>
       <c r="D6" s="29">
@@ -2141,248 +2671,330 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="30" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="30" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="27">
-        <v>20</v>
+        <f>SUMIF(E15:E26,"David",D15:D26)</f>
+        <v>23</v>
       </c>
       <c r="C7" s="28">
-        <f>B7-SUM(F15:F23)</f>
-        <v>14</v>
+        <f>B7-SUMIF(E15:E26,"David",F15:F26)</f>
+        <v>23</v>
       </c>
       <c r="D7" s="29">
         <f t="shared" ref="D7:D8" si="0">(B7-C7)/B7</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="32">
         <f>SUM(B6:B7)</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C8" s="32">
         <f>SUM(C6:C7)</f>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D8" s="29">
         <f t="shared" si="0"/>
-        <v>0.15789473684210525</v>
+        <v>0</v>
       </c>
       <c r="G8"/>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E9" s="24"/>
       <c r="G9"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E10" s="24"/>
       <c r="G10"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11" s="33"/>
       <c r="E11" s="23"/>
       <c r="F11" s="34"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="23"/>
       <c r="F12" s="34"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="33"/>
       <c r="E13" s="23"/>
       <c r="F13" s="34"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-    </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="35"/>
+    </row>
+    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="54"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-    </row>
-    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="51">
-        <v>10</v>
-      </c>
-      <c r="D15" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52">
-        <v>6</v>
-      </c>
-      <c r="G15" s="35"/>
+    </row>
+    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="58">
+        <v>4</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="51"/>
+      <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-    </row>
-    <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="59"/>
+    </row>
+    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="51"/>
       <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="24"/>
+      <c r="D16" s="58">
+        <v>4</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="51"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="59"/>
+    </row>
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="51"/>
       <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="24"/>
+      <c r="D17" s="58">
+        <v>4</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="51"/>
+      <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-    </row>
-    <row r="18" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="35"/>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="58">
+        <v>4</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-    </row>
-    <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="24"/>
+    </row>
+    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="71"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="51"/>
+      <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-    </row>
-    <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
-      <c r="B20" s="59"/>
+    </row>
+    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="51"/>
       <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="24"/>
+      <c r="D20" s="58">
+        <v>3</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-    </row>
-    <row r="21" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
-      <c r="B21" s="59"/>
+    </row>
+    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="51"/>
       <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="24"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="24"/>
-      <c r="H22"/>
-    </row>
-    <row r="23" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="59"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="24"/>
-      <c r="H23"/>
-    </row>
-    <row r="24" spans="1:11" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="5"/>
-      <c r="C24" s="47">
-        <f>SUM(C15:C23)</f>
+      <c r="D21" s="58">
+        <v>3</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="51"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="71"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="58">
+        <v>3</v>
+      </c>
+      <c r="E22" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="51"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="58">
+        <v>2</v>
+      </c>
+      <c r="E23" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="51"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+    </row>
+    <row r="24" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="58">
+        <v>2</v>
+      </c>
+      <c r="E24" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="51"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="71"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="58">
         <v>10</v>
       </c>
-      <c r="D24" s="58" t="s">
-        <v>35</v>
-      </c>
+      <c r="E25" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="51"/>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="71"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="50">
+        <v>2</v>
+      </c>
+      <c r="E26" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="51"/>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B27" s="5"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="52"/>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G30"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
+  <mergeCells count="1">
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D8">
     <cfRule type="dataBar" priority="11">
@@ -2429,7 +3041,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2453,17 +3065,17 @@
       </c>
       <c r="I1" s="16">
         <f>'Iteration 1'!B8</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M1" s="6"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H2" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="17">
         <f>'Iteration 1'!B8</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -2475,18 +3087,18 @@
         <v>3</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="14" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>17</v>
       </c>
       <c r="F4" s="9"/>
       <c r="H4" s="14"/>
       <c r="I4" s="42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2498,19 +3110,19 @@
       </c>
       <c r="C5" s="7">
         <f>SUMTASKS</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D5" s="7">
         <v>0</v>
       </c>
       <c r="E5" s="40">
         <f>C5-D5</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F5" s="2"/>
       <c r="I5" s="41">
         <f>C5</f>
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2524,511 +3136,511 @@
       </c>
       <c r="C6" s="7">
         <f>E5</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D6" s="7">
         <v>0</v>
       </c>
       <c r="E6" s="40">
         <f t="shared" ref="E6:E25" si="0">C6-D6</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2"/>
       <c r="I6" s="41">
-        <f>I5-TEAM_CAPACITY/$B$25</f>
-        <v>36.1</v>
+        <f t="shared" ref="I6:I25" si="1">I5-TEAM_CAPACITY/$B$25</f>
+        <v>38.950000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <f t="shared" ref="A7:A27" si="1">A6+1</f>
+        <f t="shared" ref="A7:A25" si="2">A6+1</f>
         <v>41357</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" ref="B7:B26" si="2">B6+1</f>
+        <f t="shared" ref="B7:B26" si="3">B6+1</f>
         <v>2</v>
       </c>
       <c r="C7" s="7">
-        <f t="shared" ref="C7:C25" si="3">E6</f>
-        <v>38</v>
+        <f t="shared" ref="C7:C25" si="4">E6</f>
+        <v>41</v>
       </c>
       <c r="D7" s="7">
         <v>0</v>
       </c>
       <c r="E7" s="40">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F7" s="2"/>
       <c r="I7" s="41">
-        <f>I6-TEAM_CAPACITY/$B$25</f>
-        <v>34.200000000000003</v>
+        <f t="shared" si="1"/>
+        <v>36.900000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41358</v>
       </c>
       <c r="B8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="C8" s="7">
-        <f t="shared" si="3"/>
-        <v>38</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D8" s="7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E8" s="40">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2"/>
       <c r="I8" s="41">
-        <f>I7-TEAM_CAPACITY/$B$25</f>
-        <v>32.300000000000004</v>
+        <f t="shared" si="1"/>
+        <v>34.850000000000009</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41359</v>
       </c>
       <c r="B9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" si="3"/>
-        <v>32</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D9" s="7">
         <v>0</v>
       </c>
       <c r="E9" s="40">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F9" s="2"/>
       <c r="I9" s="41">
-        <f>I8-TEAM_CAPACITY/$B$25</f>
-        <v>30.400000000000006</v>
+        <f t="shared" si="1"/>
+        <v>32.800000000000011</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41360</v>
       </c>
       <c r="B10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="C10" s="7">
-        <f t="shared" si="3"/>
-        <v>32</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D10" s="7">
         <v>0</v>
       </c>
       <c r="E10" s="40">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F10" s="2"/>
       <c r="I10" s="41">
-        <f>I9-TEAM_CAPACITY/$B$25</f>
-        <v>28.500000000000007</v>
+        <f t="shared" si="1"/>
+        <v>30.750000000000011</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41361</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" si="3"/>
-        <v>32</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D11" s="7">
         <v>0</v>
       </c>
       <c r="E11" s="40">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F11" s="2"/>
       <c r="I11" s="41">
-        <f>I10-TEAM_CAPACITY/$B$25</f>
-        <v>26.600000000000009</v>
+        <f t="shared" si="1"/>
+        <v>28.70000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41362</v>
       </c>
       <c r="B12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="C12" s="7">
-        <f t="shared" si="3"/>
-        <v>32</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D12" s="7">
         <v>0</v>
       </c>
       <c r="E12" s="40">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F12" s="2"/>
       <c r="I12" s="41">
-        <f>I11-TEAM_CAPACITY/$B$25</f>
-        <v>24.70000000000001</v>
+        <f t="shared" si="1"/>
+        <v>26.650000000000009</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41363</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" si="3"/>
-        <v>32</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D13" s="7">
         <v>0</v>
       </c>
       <c r="E13" s="40">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F13" s="2"/>
       <c r="I13" s="41">
-        <f>I12-TEAM_CAPACITY/$B$25</f>
-        <v>22.800000000000011</v>
+        <f t="shared" si="1"/>
+        <v>24.600000000000009</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41364</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="C14" s="7">
-        <f t="shared" si="3"/>
-        <v>32</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D14" s="7">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E14" s="40">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F14" s="2"/>
       <c r="I14" s="41">
-        <f>I13-TEAM_CAPACITY/$B$25</f>
-        <v>20.900000000000013</v>
+        <f t="shared" si="1"/>
+        <v>22.550000000000008</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
+        <f t="shared" si="2"/>
+        <v>41365</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="40">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="I15" s="41">
         <f t="shared" si="1"/>
-        <v>41365</v>
-      </c>
-      <c r="B15" s="3">
+        <v>20.500000000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="C15" s="7">
+        <v>41366</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="40">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="I16" s="41">
+        <f t="shared" si="1"/>
+        <v>18.450000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f t="shared" si="2"/>
+        <v>41367</v>
+      </c>
+      <c r="B17" s="3">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="40">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="I15" s="41">
-        <f>I14-TEAM_CAPACITY/$B$25</f>
-        <v>19.000000000000014</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <f t="shared" si="1"/>
-        <v>41366</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="C16" s="7">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="40">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="I16" s="41">
-        <f>I15-TEAM_CAPACITY/$B$25</f>
-        <v>17.100000000000016</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <f t="shared" si="1"/>
-        <v>41367</v>
-      </c>
-      <c r="B17" s="3">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
       <c r="C17" s="7">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D17" s="7">
         <v>0</v>
       </c>
       <c r="E17" s="40">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F17" s="2"/>
       <c r="I17" s="41">
-        <f>I16-TEAM_CAPACITY/$B$25</f>
-        <v>15.200000000000015</v>
+        <f t="shared" si="1"/>
+        <v>16.400000000000006</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41368</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="C18" s="7">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D18" s="7">
         <v>0</v>
       </c>
       <c r="E18" s="40">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F18" s="2"/>
       <c r="I18" s="41">
-        <f>I17-TEAM_CAPACITY/$B$25</f>
-        <v>13.300000000000015</v>
+        <f t="shared" si="1"/>
+        <v>14.350000000000005</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41369</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="C19" s="7">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D19" s="7">
         <v>0</v>
       </c>
       <c r="E19" s="40">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F19" s="2"/>
       <c r="I19" s="41">
-        <f>I18-TEAM_CAPACITY/$B$25</f>
-        <v>11.400000000000015</v>
+        <f t="shared" si="1"/>
+        <v>12.300000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41370</v>
       </c>
       <c r="B20" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D20" s="7">
         <v>0</v>
       </c>
       <c r="E20" s="40">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="I20" s="41">
-        <f>I19-TEAM_CAPACITY/$B$25</f>
-        <v>9.5000000000000142</v>
+        <f t="shared" si="1"/>
+        <v>10.250000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41371</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D21" s="7">
         <v>0</v>
       </c>
       <c r="E21" s="40">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="I21" s="41">
-        <f>I20-TEAM_CAPACITY/$B$25</f>
-        <v>7.6000000000000139</v>
+        <f t="shared" si="1"/>
+        <v>8.2000000000000028</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41372</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="C22" s="7">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D22" s="7">
         <v>0</v>
       </c>
       <c r="E22" s="40">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F22" s="11"/>
       <c r="I22" s="41">
-        <f>I21-TEAM_CAPACITY/$B$25</f>
-        <v>5.7000000000000135</v>
+        <f t="shared" si="1"/>
+        <v>6.150000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41373</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="C23" s="7">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D23" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="40">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="F23" s="11"/>
       <c r="I23" s="41">
-        <f>I22-TEAM_CAPACITY/$B$25</f>
-        <v>3.8000000000000136</v>
+        <f t="shared" si="1"/>
+        <v>4.1000000000000032</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41374</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="C24" s="7">
-        <f t="shared" si="3"/>
-        <v>11</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D24" s="7">
         <v>0</v>
       </c>
       <c r="E24" s="40">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="F24" s="11"/>
       <c r="I24" s="41">
-        <f>I23-TEAM_CAPACITY/$B$25</f>
-        <v>1.9000000000000137</v>
+        <f t="shared" si="1"/>
+        <v>2.0500000000000034</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41375</v>
       </c>
       <c r="B25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="C25" s="7">
-        <f t="shared" si="3"/>
-        <v>11</v>
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="D25" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E25" s="40">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="F25" s="11"/>
       <c r="I25" s="41">
-        <f>I24-TEAM_CAPACITY/$B$25</f>
-        <v>1.3766765505351941E-14</v>
+        <f t="shared" si="1"/>
+        <v>3.5527136788005009E-15</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3036,12 +3648,12 @@
         <v>2</v>
       </c>
       <c r="B26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="C26" s="7">
         <f>E25</f>
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="D26" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
update burndown, initial documentation
</commit_message>
<xml_diff>
--- a/prjplanning/projektplanung.xlsx
+++ b/prjplanning/projektplanung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="24240" windowHeight="13680"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="24240" windowHeight="13680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="5" r:id="rId1"/>
@@ -805,83 +805,83 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1089,46 +1089,46 @@
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1294,11 +1294,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85031936"/>
-        <c:axId val="85041920"/>
+        <c:axId val="92969984"/>
+        <c:axId val="92979968"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="85031936"/>
+        <c:axId val="92969984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1318,7 +1318,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85041920"/>
+        <c:crossAx val="92979968"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="0"/>
@@ -1329,7 +1329,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="85041920"/>
+        <c:axId val="92979968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1361,7 +1361,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85031936"/>
+        <c:crossAx val="92969984"/>
         <c:crossesAt val="41221"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -2088,7 +2088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2172,18 +2172,18 @@
       <c r="E7" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="67" t="s">
+      <c r="G7" s="61" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="72">
+      <c r="B8" s="65">
         <v>1</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="66" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="27">
@@ -2192,19 +2192,19 @@
       <c r="E8" s="27">
         <v>23</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="62">
         <f>SUM(D8:E8)</f>
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="74">
+      <c r="B9" s="67">
         <v>2</v>
       </c>
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="68" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="27">
@@ -2213,10 +2213,10 @@
       <c r="E9" s="27">
         <v>15</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="F9" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="68">
+      <c r="G9" s="62">
         <f t="shared" ref="G9:G11" si="0">SUM(D9:E9)</f>
         <v>20</v>
       </c>
@@ -2234,8 +2234,8 @@
       <c r="E10" s="48">
         <v>22</v>
       </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="68">
+      <c r="F10" s="53"/>
+      <c r="G10" s="62">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
@@ -2249,7 +2249,7 @@
         <f>SUM(E8:E10)</f>
         <v>60</v>
       </c>
-      <c r="G11" s="68">
+      <c r="G11" s="62">
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
@@ -2264,11 +2264,11 @@
       <c r="B15" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
       <c r="F15" s="38" t="s">
         <v>39</v>
       </c>
@@ -2277,15 +2277,15 @@
       <c r="B16" s="44">
         <v>1</v>
       </c>
-      <c r="C16" s="76" t="s">
+      <c r="C16" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="58">
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="54">
         <v>8</v>
       </c>
-      <c r="G16" s="59" t="s">
+      <c r="G16" s="55" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2293,12 +2293,12 @@
       <c r="B17" s="44">
         <v>2</v>
       </c>
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="58">
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="54">
         <v>8</v>
       </c>
       <c r="G17" s="24" t="s">
@@ -2309,12 +2309,12 @@
       <c r="B18" s="44">
         <v>3</v>
       </c>
-      <c r="C18" s="76" t="s">
+      <c r="C18" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="58" t="s">
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="54" t="s">
         <v>40</v>
       </c>
       <c r="G18" s="24"/>
@@ -2324,15 +2324,15 @@
       <c r="B19" s="44">
         <v>4</v>
       </c>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="58">
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="54">
         <v>6</v>
       </c>
-      <c r="G19" s="62" t="s">
+      <c r="G19" s="56" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2340,12 +2340,12 @@
       <c r="B20" s="44">
         <v>5</v>
       </c>
-      <c r="C20" s="76" t="s">
+      <c r="C20" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="58">
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="54">
         <v>3</v>
       </c>
       <c r="G20" s="24"/>
@@ -2354,12 +2354,12 @@
       <c r="B21" s="44">
         <v>5</v>
       </c>
-      <c r="C21" s="76" t="s">
+      <c r="C21" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="58">
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="54">
         <v>2</v>
       </c>
       <c r="G21" s="24"/>
@@ -2368,12 +2368,12 @@
       <c r="B22" s="44">
         <v>6</v>
       </c>
-      <c r="C22" s="76" t="s">
+      <c r="C22" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="58">
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="54">
         <v>2</v>
       </c>
       <c r="G22" s="24"/>
@@ -2382,12 +2382,12 @@
       <c r="B23" s="44">
         <v>7</v>
       </c>
-      <c r="C23" s="78" t="s">
+      <c r="C23" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="58">
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="54">
         <v>20</v>
       </c>
       <c r="G23" s="24"/>
@@ -2396,12 +2396,12 @@
       <c r="B24" s="44">
         <v>7</v>
       </c>
-      <c r="C24" s="76" t="s">
+      <c r="C24" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="58">
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="54">
         <v>10</v>
       </c>
       <c r="G24" s="24"/>
@@ -2412,12 +2412,12 @@
       <c r="B25" s="44">
         <v>8</v>
       </c>
-      <c r="C25" s="76" t="s">
+      <c r="C25" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="58">
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="54">
         <v>2</v>
       </c>
       <c r="G25" s="24"/>
@@ -2426,12 +2426,12 @@
       <c r="B26" s="44">
         <v>9</v>
       </c>
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="58">
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="54">
         <v>10</v>
       </c>
       <c r="G26" s="24"/>
@@ -2440,12 +2440,12 @@
       <c r="B27" s="44">
         <v>10</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="58">
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="54">
         <v>4</v>
       </c>
       <c r="G27" s="24" t="s">
@@ -2456,12 +2456,12 @@
       <c r="B28" s="44">
         <v>11</v>
       </c>
-      <c r="C28" s="60" t="s">
+      <c r="C28" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="58">
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="54">
         <v>10</v>
       </c>
       <c r="G28" s="24"/>
@@ -2471,12 +2471,12 @@
       <c r="B29" s="44">
         <v>12</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="58">
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="54">
         <v>4</v>
       </c>
       <c r="G29" s="24"/>
@@ -2485,12 +2485,12 @@
       <c r="B30" s="44">
         <v>13</v>
       </c>
-      <c r="C30" s="60" t="s">
+      <c r="C30" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="61"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="58">
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="54">
         <v>5</v>
       </c>
       <c r="G30" s="24"/>
@@ -2499,12 +2499,12 @@
       <c r="B31" s="44">
         <v>14</v>
       </c>
-      <c r="C31" s="60" t="s">
+      <c r="C31" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="58">
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="54">
         <v>3</v>
       </c>
       <c r="G31" s="24" t="s">
@@ -2515,12 +2515,12 @@
       <c r="B32" s="44">
         <v>15</v>
       </c>
-      <c r="C32" s="60" t="s">
+      <c r="C32" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="58">
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="54">
         <v>6</v>
       </c>
       <c r="G32" t="s">
@@ -2531,32 +2531,32 @@
       <c r="B33" s="44">
         <v>16</v>
       </c>
-      <c r="C33" s="60" t="s">
+      <c r="C33" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="58">
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="54">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="2:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E35" s="64" t="s">
+      <c r="E35" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="63">
+      <c r="F35" s="57">
         <f>SUM(F16:F33)</f>
         <v>113</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
@@ -2565,12 +2565,12 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
     <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2582,7 +2582,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2645,7 +2645,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="38" t="s">
         <v>61</v>
@@ -2663,12 +2663,12 @@
         <v>18</v>
       </c>
       <c r="C6" s="28">
-        <f>B6-SUMIF(E14:E25,"Roger",F14:F25)</f>
-        <v>18</v>
+        <f>B6-SUMIF(E15:E26,"Roger",F15:F26)</f>
+        <v>10</v>
       </c>
       <c r="D6" s="29">
         <f>(B6-C6)/B6</f>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="30" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2681,11 +2681,11 @@
       </c>
       <c r="C7" s="28">
         <f>B7-SUMIF(E15:E26,"David",F15:F26)</f>
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D7" s="29">
         <f t="shared" ref="D7:D8" si="0">(B7-C7)/B7</f>
-        <v>0</v>
+        <v>0.30434782608695654</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -2698,11 +2698,11 @@
       </c>
       <c r="C8" s="32">
         <f>SUM(C6:C7)</f>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D8" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.36585365853658536</v>
       </c>
       <c r="G8"/>
     </row>
@@ -2748,11 +2748,11 @@
       <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="69"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="49" t="s">
         <v>13</v>
       </c>
@@ -2773,13 +2773,15 @@
       </c>
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
-      <c r="D15" s="58">
+      <c r="D15" s="54">
         <v>4</v>
       </c>
       <c r="E15" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="51"/>
+      <c r="F15" s="51">
+        <v>3</v>
+      </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
@@ -2791,13 +2793,15 @@
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
-      <c r="D16" s="58">
+      <c r="D16" s="54">
         <v>4</v>
       </c>
       <c r="E16" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="51"/>
+      <c r="F16" s="51">
+        <v>4</v>
+      </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
@@ -2809,13 +2813,15 @@
       </c>
       <c r="B17" s="51"/>
       <c r="C17" s="51"/>
-      <c r="D17" s="58">
+      <c r="D17" s="54">
         <v>4</v>
       </c>
       <c r="E17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="51"/>
+      <c r="F17" s="51">
+        <v>2</v>
+      </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
@@ -2827,13 +2833,15 @@
       </c>
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
-      <c r="D18" s="58">
+      <c r="D18" s="54">
         <v>4</v>
       </c>
       <c r="E18" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="51"/>
+      <c r="F18" s="51">
+        <v>2</v>
+      </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
@@ -2843,15 +2851,17 @@
       <c r="A19" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="58" t="s">
+      <c r="B19" s="64"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="54" t="s">
         <v>40</v>
       </c>
       <c r="E19" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="51"/>
+      <c r="F19" s="51">
+        <v>1</v>
+      </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
@@ -2863,7 +2873,7 @@
       </c>
       <c r="B20" s="51"/>
       <c r="C20" s="51"/>
-      <c r="D20" s="58">
+      <c r="D20" s="54">
         <v>3</v>
       </c>
       <c r="E20" s="51" t="s">
@@ -2881,7 +2891,7 @@
       </c>
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
-      <c r="D21" s="58">
+      <c r="D21" s="54">
         <v>3</v>
       </c>
       <c r="E21" s="51" t="s">
@@ -2897,9 +2907,9 @@
       <c r="A22" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="58">
+      <c r="B22" s="64"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="54">
         <v>3</v>
       </c>
       <c r="E22" s="51" t="s">
@@ -2917,13 +2927,15 @@
       </c>
       <c r="B23" s="51"/>
       <c r="C23" s="51"/>
-      <c r="D23" s="58">
+      <c r="D23" s="54">
         <v>2</v>
       </c>
       <c r="E23" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="51"/>
+      <c r="F23" s="51">
+        <v>1</v>
+      </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
@@ -2935,7 +2947,7 @@
       </c>
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
-      <c r="D24" s="58">
+      <c r="D24" s="54">
         <v>2</v>
       </c>
       <c r="E24" s="51" t="s">
@@ -2951,9 +2963,9 @@
       <c r="A25" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="58">
+      <c r="B25" s="64"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="54">
         <v>10</v>
       </c>
       <c r="E25" s="51" t="s">
@@ -2966,15 +2978,17 @@
       <c r="A26" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="71"/>
-      <c r="C26" s="70"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="63"/>
       <c r="D26" s="50">
         <v>2</v>
       </c>
       <c r="E26" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="51"/>
+      <c r="F26" s="51">
+        <v>2</v>
+      </c>
       <c r="G26"/>
     </row>
     <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -3040,9 +3054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3295,11 +3307,11 @@
         <v>41</v>
       </c>
       <c r="D12" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E12" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F12" s="2"/>
       <c r="I12" s="41">
@@ -3318,14 +3330,14 @@
       </c>
       <c r="C13" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D13" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E13" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F13" s="2"/>
       <c r="I13" s="41">
@@ -3344,14 +3356,14 @@
       </c>
       <c r="C14" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D14" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E14" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F14" s="2"/>
       <c r="I14" s="41">
@@ -3370,14 +3382,14 @@
       </c>
       <c r="C15" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D15" s="7">
         <v>0</v>
       </c>
       <c r="E15" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F15" s="2"/>
       <c r="I15" s="41">
@@ -3396,14 +3408,14 @@
       </c>
       <c r="C16" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D16" s="7">
         <v>0</v>
       </c>
       <c r="E16" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F16" s="2"/>
       <c r="I16" s="41">
@@ -3422,14 +3434,14 @@
       </c>
       <c r="C17" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D17" s="7">
         <v>0</v>
       </c>
       <c r="E17" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F17" s="2"/>
       <c r="I17" s="41">
@@ -3448,14 +3460,14 @@
       </c>
       <c r="C18" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D18" s="7">
         <v>0</v>
       </c>
       <c r="E18" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F18" s="2"/>
       <c r="I18" s="41">
@@ -3474,14 +3486,14 @@
       </c>
       <c r="C19" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D19" s="7">
         <v>0</v>
       </c>
       <c r="E19" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F19" s="2"/>
       <c r="I19" s="41">
@@ -3500,14 +3512,14 @@
       </c>
       <c r="C20" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D20" s="7">
         <v>0</v>
       </c>
       <c r="E20" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="I20" s="41">
         <f t="shared" si="1"/>
@@ -3525,14 +3537,14 @@
       </c>
       <c r="C21" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D21" s="7">
         <v>0</v>
       </c>
       <c r="E21" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="I21" s="41">
         <f t="shared" si="1"/>
@@ -3550,14 +3562,14 @@
       </c>
       <c r="C22" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D22" s="7">
         <v>0</v>
       </c>
       <c r="E22" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F22" s="11"/>
       <c r="I22" s="41">
@@ -3576,14 +3588,14 @@
       </c>
       <c r="C23" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D23" s="7">
         <v>0</v>
       </c>
       <c r="E23" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F23" s="11"/>
       <c r="I23" s="41">
@@ -3602,14 +3614,14 @@
       </c>
       <c r="C24" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D24" s="7">
         <v>0</v>
       </c>
       <c r="E24" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F24" s="11"/>
       <c r="I24" s="41">
@@ -3628,14 +3640,14 @@
       </c>
       <c r="C25" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D25" s="7">
         <v>0</v>
       </c>
       <c r="E25" s="40">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F25" s="11"/>
       <c r="I25" s="41">
@@ -3653,7 +3665,7 @@
       </c>
       <c r="C26" s="7">
         <f>E25</f>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D26" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
implemented persistence of cultures
</commit_message>
<xml_diff>
--- a/prjplanning/projektplanung.xlsx
+++ b/prjplanning/projektplanung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="24240" windowHeight="13680" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="24240" windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="5" r:id="rId1"/>
@@ -880,28 +880,28 @@
     <xf numFmtId="164" fontId="9" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1323,11 +1323,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94731264"/>
-        <c:axId val="94741248"/>
+        <c:axId val="94674944"/>
+        <c:axId val="94676480"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="94731264"/>
+        <c:axId val="94674944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,7 +1347,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94741248"/>
+        <c:crossAx val="94676480"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="0"/>
@@ -1358,7 +1358,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="94741248"/>
+        <c:axId val="94676480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1390,7 +1390,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94731264"/>
+        <c:crossAx val="94674944"/>
         <c:crossesAt val="41221"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -1584,67 +1584,67 @@
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>48</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>48</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>48</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>48</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>48</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>48</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>48</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>48</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>48</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>48</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>48</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1810,11 +1810,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="56574336"/>
-        <c:axId val="56575872"/>
+        <c:axId val="106562688"/>
+        <c:axId val="106564224"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="56574336"/>
+        <c:axId val="106562688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,7 +1834,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56575872"/>
+        <c:crossAx val="106564224"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="0"/>
@@ -1845,7 +1845,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="56575872"/>
+        <c:axId val="106564224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1877,7 +1877,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56574336"/>
+        <c:crossAx val="106562688"/>
         <c:crossesAt val="41221"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -3007,10 +3007,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:F29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3185,11 +3188,11 @@
       <c r="B15" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
       <c r="F15" s="38" t="s">
         <v>39</v>
       </c>
@@ -3198,11 +3201,11 @@
       <c r="B16" s="44">
         <v>1</v>
       </c>
-      <c r="C16" s="71" t="s">
+      <c r="C16" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
       <c r="F16" s="54">
         <v>8</v>
       </c>
@@ -3214,11 +3217,11 @@
       <c r="B17" s="44">
         <v>2</v>
       </c>
-      <c r="C17" s="71" t="s">
+      <c r="C17" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="54">
         <v>8</v>
       </c>
@@ -3230,11 +3233,11 @@
       <c r="B18" s="44">
         <v>3</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
       <c r="F18" s="54" t="s">
         <v>40</v>
       </c>
@@ -3245,11 +3248,11 @@
       <c r="B19" s="44">
         <v>4</v>
       </c>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
       <c r="F19" s="54">
         <v>6</v>
       </c>
@@ -3261,11 +3264,11 @@
       <c r="B20" s="44">
         <v>5</v>
       </c>
-      <c r="C20" s="71" t="s">
+      <c r="C20" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
       <c r="F20" s="54">
         <v>3</v>
       </c>
@@ -3275,11 +3278,11 @@
       <c r="B21" s="44">
         <v>5</v>
       </c>
-      <c r="C21" s="71" t="s">
+      <c r="C21" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
       <c r="F21" s="54">
         <v>2</v>
       </c>
@@ -3289,11 +3292,11 @@
       <c r="B22" s="44">
         <v>6</v>
       </c>
-      <c r="C22" s="71" t="s">
+      <c r="C22" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
       <c r="F22" s="54">
         <v>2</v>
       </c>
@@ -3303,11 +3306,11 @@
       <c r="B23" s="44">
         <v>7</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
       <c r="F23" s="54">
         <v>20</v>
       </c>
@@ -3317,11 +3320,11 @@
       <c r="B24" s="44">
         <v>7</v>
       </c>
-      <c r="C24" s="71" t="s">
+      <c r="C24" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
       <c r="F24" s="54">
         <v>10</v>
       </c>
@@ -3333,39 +3336,39 @@
       <c r="B25" s="44">
         <v>8</v>
       </c>
-      <c r="C25" s="71" t="s">
+      <c r="C25" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
       <c r="F25" s="54">
         <v>2</v>
       </c>
       <c r="G25" s="24"/>
     </row>
-    <row r="26" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="44">
         <v>9</v>
       </c>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
       <c r="F26" s="54">
         <v>10</v>
       </c>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="44">
         <v>10</v>
       </c>
-      <c r="C27" s="69" t="s">
+      <c r="C27" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
       <c r="F27" s="54">
         <v>4</v>
       </c>
@@ -3377,40 +3380,40 @@
       <c r="B28" s="44">
         <v>11</v>
       </c>
-      <c r="C28" s="69" t="s">
+      <c r="C28" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
       <c r="F28" s="54">
         <v>10</v>
       </c>
       <c r="G28" s="24"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="44">
         <v>12</v>
       </c>
-      <c r="C29" s="69" t="s">
+      <c r="C29" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
       <c r="F29" s="54">
         <v>4</v>
       </c>
       <c r="G29" s="24"/>
     </row>
-    <row r="30" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="44">
         <v>13</v>
       </c>
-      <c r="C30" s="69" t="s">
+      <c r="C30" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
       <c r="F30" s="54">
         <v>5</v>
       </c>
@@ -3420,11 +3423,11 @@
       <c r="B31" s="44">
         <v>14</v>
       </c>
-      <c r="C31" s="69" t="s">
+      <c r="C31" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
       <c r="F31" s="54">
         <v>3</v>
       </c>
@@ -3436,11 +3439,11 @@
       <c r="B32" s="44">
         <v>15</v>
       </c>
-      <c r="C32" s="69" t="s">
+      <c r="C32" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
       <c r="F32" s="54">
         <v>6</v>
       </c>
@@ -3452,11 +3455,11 @@
       <c r="B33" s="44">
         <v>16</v>
       </c>
-      <c r="C33" s="69" t="s">
+      <c r="C33" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
       <c r="F33" s="54">
         <v>10</v>
       </c>
@@ -3473,16 +3476,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="C24:E24"/>
@@ -3492,9 +3485,19 @@
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4648,8 +4651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4998,7 +5001,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5068,11 +5071,11 @@
         <v>48</v>
       </c>
       <c r="D5" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" s="40">
         <f>C5-D5</f>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" s="2"/>
       <c r="I5" s="41">
@@ -5091,14 +5094,14 @@
       </c>
       <c r="C6" s="7">
         <f>E5</f>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D6" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" s="40">
         <f t="shared" ref="E6:E25" si="0">C6-D6</f>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2"/>
       <c r="I6" s="41">
@@ -5117,14 +5120,14 @@
       </c>
       <c r="C7" s="7">
         <f t="shared" ref="C7:C25" si="3">E6</f>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D7" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F7" s="2"/>
       <c r="I7" s="41">
@@ -5143,14 +5146,14 @@
       </c>
       <c r="C8" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D8" s="7">
         <v>0</v>
       </c>
       <c r="E8" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F8" s="2"/>
       <c r="I8" s="41">
@@ -5169,14 +5172,14 @@
       </c>
       <c r="C9" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D9" s="7">
         <v>0</v>
       </c>
       <c r="E9" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F9" s="2"/>
       <c r="I9" s="41">
@@ -5195,14 +5198,14 @@
       </c>
       <c r="C10" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D10" s="7">
         <v>0</v>
       </c>
       <c r="E10" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2"/>
       <c r="I10" s="41">
@@ -5221,14 +5224,14 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D11" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F11" s="2"/>
       <c r="I11" s="41">
@@ -5247,14 +5250,14 @@
       </c>
       <c r="C12" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D12" s="7">
         <v>0</v>
       </c>
       <c r="E12" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F12" s="2"/>
       <c r="I12" s="41">
@@ -5273,14 +5276,14 @@
       </c>
       <c r="C13" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D13" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E13" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F13" s="2"/>
       <c r="I13" s="41">
@@ -5299,14 +5302,14 @@
       </c>
       <c r="C14" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D14" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E14" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F14" s="2"/>
       <c r="I14" s="41">
@@ -5325,14 +5328,14 @@
       </c>
       <c r="C15" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D15" s="7">
         <v>0</v>
       </c>
       <c r="E15" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F15" s="2"/>
       <c r="I15" s="41">
@@ -5351,14 +5354,14 @@
       </c>
       <c r="C16" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D16" s="7">
         <v>0</v>
       </c>
       <c r="E16" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F16" s="2"/>
       <c r="I16" s="41">
@@ -5377,14 +5380,14 @@
       </c>
       <c r="C17" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D17" s="7">
         <v>0</v>
       </c>
       <c r="E17" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F17" s="2"/>
       <c r="I17" s="41">
@@ -5403,14 +5406,14 @@
       </c>
       <c r="C18" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D18" s="7">
         <v>0</v>
       </c>
       <c r="E18" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F18" s="2"/>
       <c r="I18" s="41">
@@ -5429,14 +5432,14 @@
       </c>
       <c r="C19" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D19" s="7">
         <v>0</v>
       </c>
       <c r="E19" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F19" s="2"/>
       <c r="I19" s="41">
@@ -5455,14 +5458,14 @@
       </c>
       <c r="C20" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D20" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E20" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="I20" s="41">
         <f t="shared" si="1"/>
@@ -5480,14 +5483,14 @@
       </c>
       <c r="C21" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D21" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E21" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="I21" s="41">
         <f t="shared" si="1"/>
@@ -5505,14 +5508,14 @@
       </c>
       <c r="C22" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="D22" s="7">
         <v>0</v>
       </c>
       <c r="E22" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F22" s="11"/>
       <c r="I22" s="41">
@@ -5531,14 +5534,14 @@
       </c>
       <c r="C23" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="D23" s="7">
         <v>0</v>
       </c>
       <c r="E23" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F23" s="11"/>
       <c r="I23" s="41">
@@ -5557,14 +5560,14 @@
       </c>
       <c r="C24" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="D24" s="7">
         <v>0</v>
       </c>
       <c r="E24" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F24" s="11"/>
       <c r="I24" s="41">
@@ -5583,14 +5586,14 @@
       </c>
       <c r="C25" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="D25" s="7">
         <v>0</v>
       </c>
       <c r="E25" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F25" s="11"/>
       <c r="I25" s="41">
@@ -5608,7 +5611,7 @@
       </c>
       <c r="C26" s="7">
         <f>E25</f>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="D26" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
updated documentation and prjplanning
</commit_message>
<xml_diff>
--- a/prjplanning/projektplanung.xlsx
+++ b/prjplanning/projektplanung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="24240" windowHeight="13680" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="24240" windowHeight="13680" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="5" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="73">
   <si>
     <t xml:space="preserve"> Tag</t>
   </si>
@@ -284,6 +284,9 @@
   <si>
     <t>Tests implementieren und Dokumentieren</t>
   </si>
+  <si>
+    <t>Dokumentation nachführen - Teil 3</t>
+  </si>
 </sst>
 </file>
 
@@ -481,7 +484,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -736,22 +739,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -917,15 +909,6 @@
     <xf numFmtId="164" fontId="9" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -944,6 +927,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -952,9 +941,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1366,11 +1352,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82354944"/>
-        <c:axId val="82356480"/>
+        <c:axId val="80319616"/>
+        <c:axId val="80321152"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="82354944"/>
+        <c:axId val="80319616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1390,7 +1376,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82356480"/>
+        <c:crossAx val="80321152"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="0"/>
@@ -1401,7 +1387,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="82356480"/>
+        <c:axId val="80321152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1433,7 +1419,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82354944"/>
+        <c:crossAx val="80319616"/>
         <c:crossesAt val="41221"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -1853,11 +1839,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95438720"/>
-        <c:axId val="95440256"/>
+        <c:axId val="84228352"/>
+        <c:axId val="84234240"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="95438720"/>
+        <c:axId val="84228352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1877,7 +1863,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95440256"/>
+        <c:crossAx val="84234240"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="0"/>
@@ -1888,7 +1874,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="95440256"/>
+        <c:axId val="84234240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1920,7 +1906,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95438720"/>
+        <c:crossAx val="84228352"/>
         <c:crossesAt val="41221"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -2114,73 +2100,73 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>45</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>45</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>45</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>45</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>45</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>45</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>45</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>45</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2272,70 +2258,70 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>33.32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>31.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46</c:v>
+                  <c:v>29.96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44</c:v>
+                  <c:v>28.28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42</c:v>
+                  <c:v>26.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>24.92</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38</c:v>
+                  <c:v>23.240000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
+                  <c:v>21.560000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34</c:v>
+                  <c:v>19.880000000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32</c:v>
+                  <c:v>18.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30</c:v>
+                  <c:v>16.520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>14.840000000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>13.160000000000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24</c:v>
+                  <c:v>11.480000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22</c:v>
+                  <c:v>9.8000000000000043</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20</c:v>
+                  <c:v>8.1200000000000045</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>6.4400000000000048</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16</c:v>
+                  <c:v>4.7600000000000051</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14</c:v>
+                  <c:v>3.0800000000000054</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12</c:v>
+                  <c:v>1.4000000000000055</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10</c:v>
+                  <c:v>-0.27999999999999448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2352,11 +2338,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94890240"/>
-        <c:axId val="94961664"/>
+        <c:axId val="86239872"/>
+        <c:axId val="86245760"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="94890240"/>
+        <c:axId val="86239872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2376,7 +2362,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94961664"/>
+        <c:crossAx val="86245760"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="0"/>
@@ -2387,7 +2373,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="94961664"/>
+        <c:axId val="86245760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2419,7 +2405,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94890240"/>
+        <c:crossAx val="86239872"/>
         <c:crossesAt val="41221"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -3346,12 +3332,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.5693</cdr:x>
-      <cdr:y>0.20093</cdr:y>
+      <cdr:x>0.50508</cdr:x>
+      <cdr:y>0.78476</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.76926</cdr:x>
-      <cdr:y>0.25029</cdr:y>
+      <cdr:x>0.70504</cdr:x>
+      <cdr:y>0.83412</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3360,7 +3346,7 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5562935" y="1353638"/>
+          <a:off x="4935401" y="5286926"/>
           <a:ext cx="1953914" cy="332537"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="roundRect">
@@ -3506,12 +3492,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.08636</cdr:x>
-      <cdr:y>0.32726</cdr:y>
+      <cdr:x>0.72742</cdr:x>
+      <cdr:y>0.59672</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.27205</cdr:x>
-      <cdr:y>0.38469</cdr:y>
+      <cdr:x>0.91311</cdr:x>
+      <cdr:y>0.65415</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3520,8 +3506,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="843836" y="2204768"/>
-          <a:ext cx="1814475" cy="386905"/>
+          <a:off x="7107957" y="4020096"/>
+          <a:ext cx="1814475" cy="386904"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="roundRect">
           <a:avLst/>
@@ -4135,11 +4121,11 @@
       <c r="B15" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="76" t="s">
+      <c r="C15" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
       <c r="F15" s="38" t="s">
         <v>39</v>
       </c>
@@ -4148,11 +4134,11 @@
       <c r="B16" s="44">
         <v>1</v>
       </c>
-      <c r="C16" s="72" t="s">
+      <c r="C16" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
       <c r="F16" s="54">
         <v>8</v>
       </c>
@@ -4164,11 +4150,11 @@
       <c r="B17" s="44">
         <v>2</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="54">
         <v>8</v>
       </c>
@@ -4180,11 +4166,11 @@
       <c r="B18" s="44">
         <v>3</v>
       </c>
-      <c r="C18" s="72" t="s">
+      <c r="C18" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
       <c r="F18" s="54" t="s">
         <v>40</v>
       </c>
@@ -4195,11 +4181,11 @@
       <c r="B19" s="44">
         <v>4</v>
       </c>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
       <c r="F19" s="54">
         <v>6</v>
       </c>
@@ -4211,11 +4197,11 @@
       <c r="B20" s="44">
         <v>5</v>
       </c>
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
       <c r="F20" s="54">
         <v>3</v>
       </c>
@@ -4225,11 +4211,11 @@
       <c r="B21" s="44">
         <v>5</v>
       </c>
-      <c r="C21" s="72" t="s">
+      <c r="C21" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
       <c r="F21" s="54">
         <v>2</v>
       </c>
@@ -4239,11 +4225,11 @@
       <c r="B22" s="44">
         <v>6</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
       <c r="F22" s="54">
         <v>2</v>
       </c>
@@ -4253,11 +4239,11 @@
       <c r="B23" s="44">
         <v>7</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
       <c r="F23" s="54">
         <v>20</v>
       </c>
@@ -4267,11 +4253,11 @@
       <c r="B24" s="44">
         <v>7</v>
       </c>
-      <c r="C24" s="72" t="s">
+      <c r="C24" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
       <c r="F24" s="54">
         <v>10</v>
       </c>
@@ -4283,11 +4269,11 @@
       <c r="B25" s="44">
         <v>8</v>
       </c>
-      <c r="C25" s="72" t="s">
+      <c r="C25" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
       <c r="F25" s="54">
         <v>2</v>
       </c>
@@ -4297,11 +4283,11 @@
       <c r="B26" s="44">
         <v>9</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
       <c r="F26" s="54">
         <v>10</v>
       </c>
@@ -4311,11 +4297,11 @@
       <c r="B27" s="44">
         <v>10</v>
       </c>
-      <c r="C27" s="74" t="s">
+      <c r="C27" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
       <c r="F27" s="54">
         <v>4</v>
       </c>
@@ -4327,11 +4313,11 @@
       <c r="B28" s="44">
         <v>11</v>
       </c>
-      <c r="C28" s="74" t="s">
+      <c r="C28" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
       <c r="F28" s="54">
         <v>10</v>
       </c>
@@ -4342,11 +4328,11 @@
       <c r="B29" s="44">
         <v>12</v>
       </c>
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
       <c r="F29" s="54">
         <v>4</v>
       </c>
@@ -4356,11 +4342,11 @@
       <c r="B30" s="44">
         <v>13</v>
       </c>
-      <c r="C30" s="70" t="s">
+      <c r="C30" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
       <c r="F30" s="54">
         <v>5</v>
       </c>
@@ -4370,11 +4356,11 @@
       <c r="B31" s="44">
         <v>14</v>
       </c>
-      <c r="C31" s="70" t="s">
+      <c r="C31" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
       <c r="F31" s="54">
         <v>3</v>
       </c>
@@ -4386,11 +4372,11 @@
       <c r="B32" s="44">
         <v>15</v>
       </c>
-      <c r="C32" s="70" t="s">
+      <c r="C32" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="71"/>
-      <c r="E32" s="71"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
       <c r="F32" s="54">
         <v>6</v>
       </c>
@@ -4402,11 +4388,11 @@
       <c r="B33" s="44">
         <v>16</v>
       </c>
-      <c r="C33" s="70" t="s">
+      <c r="C33" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
       <c r="F33" s="54">
         <v>10</v>
       </c>
@@ -4423,16 +4409,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="C24:E24"/>
@@ -4442,6 +4418,16 @@
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
@@ -4619,11 +4605,11 @@
       <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="80"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="49" t="s">
         <v>13</v>
       </c>
@@ -5598,8 +5584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5765,11 +5751,11 @@
       <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="80"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="49" t="s">
         <v>13</v>
       </c>
@@ -6604,10 +6590,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6670,15 +6656,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="27">
-        <v>30</v>
+        <f>SUMIF(E15:E24,"Roger",D15:D24)</f>
+        <v>19</v>
       </c>
       <c r="C6" s="28">
-        <f>B6-SUMIF(E15:E22,"Roger",F15:F22)</f>
-        <v>23</v>
+        <f>B6-SUMIF(E15:E24,"Roger",F15:F24)</f>
+        <v>0</v>
       </c>
       <c r="D6" s="29">
         <f>(B6-C6)/B6</f>
-        <v>0.23333333333333334</v>
+        <v>1</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
@@ -6688,15 +6675,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="27">
-        <v>22</v>
+        <f>SUMIF(E15:E24,"David",D15:D24)</f>
+        <v>16</v>
       </c>
       <c r="C7" s="28">
-        <f>B7-SUMIF(E15:E22,"David",F15:F22)</f>
-        <v>22</v>
+        <f>B7-SUMIF(E15:E24,"David",F15:F24)</f>
+        <v>0</v>
       </c>
       <c r="D7" s="29">
         <f t="shared" ref="D7:D8" si="0">(B7-C7)/B7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -6707,15 +6695,15 @@
       </c>
       <c r="B8" s="32">
         <f>SUM(B6:B7)</f>
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C8" s="32">
         <f>SUM(C6:C7)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="D8" s="29">
         <f t="shared" si="0"/>
-        <v>0.13461538461538461</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -6745,11 +6733,11 @@
       <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="80"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="49" t="s">
         <v>13</v>
       </c>
@@ -6761,11 +6749,11 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="54">
         <v>5</v>
       </c>
@@ -6773,31 +6761,31 @@
         <v>60</v>
       </c>
       <c r="F15" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
       <c r="D16" s="54">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E16" s="51" t="s">
         <v>60</v>
       </c>
       <c r="F16" s="51">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
       <c r="D17" s="54">
         <v>6</v>
       </c>
@@ -6805,15 +6793,15 @@
         <v>34</v>
       </c>
       <c r="F17" s="51">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
       <c r="D18" s="54">
         <v>3</v>
       </c>
@@ -6821,15 +6809,15 @@
         <v>60</v>
       </c>
       <c r="F18" s="51">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
       <c r="D19" s="54">
         <v>1</v>
       </c>
@@ -6837,15 +6825,15 @@
         <v>60</v>
       </c>
       <c r="F19" s="51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
       <c r="D20" s="54">
         <v>2</v>
       </c>
@@ -6853,15 +6841,15 @@
         <v>34</v>
       </c>
       <c r="F20" s="51">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
       <c r="D21" s="54">
         <v>2</v>
       </c>
@@ -6869,15 +6857,15 @@
         <v>60</v>
       </c>
       <c r="F21" s="51">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
       <c r="D22" s="54">
         <v>2</v>
       </c>
@@ -6885,35 +6873,54 @@
         <v>60</v>
       </c>
       <c r="F22" s="51">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="81" t="s">
+      <c r="B23" s="76"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="54">
+        <v>2</v>
+      </c>
+      <c r="E23" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="81">
+      <c r="F23" s="51">
         <v>2</v>
       </c>
     </row>
+    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="76"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="54">
+        <v>6</v>
+      </c>
+      <c r="E24" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="51">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D8">
     <cfRule type="dataBar" priority="1">
@@ -6958,8 +6965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6982,7 +6989,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="16">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="M1" s="6"/>
     </row>
@@ -6991,7 +6998,7 @@
         <v>17</v>
       </c>
       <c r="I2" s="17">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -7025,18 +7032,17 @@
         <v>0</v>
       </c>
       <c r="C5" s="7">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D5" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E5" s="40">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2"/>
       <c r="I5" s="41">
-        <f>C5</f>
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -7050,433 +7056,433 @@
       </c>
       <c r="C6" s="7">
         <f>E5</f>
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D6" s="7">
         <v>4</v>
       </c>
       <c r="E6" s="40">
         <f t="shared" ref="E6:E26" si="0">C6-D6</f>
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2"/>
       <c r="I6" s="41">
-        <f t="shared" ref="I6:I26" si="1">I5-TEAM_CAPACITY/$B$26</f>
-        <v>50</v>
+        <f>I5-TEAM_CAPACITY/$B$26</f>
+        <v>33.32</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <f t="shared" ref="A7:B22" si="2">A6+1</f>
+        <f t="shared" ref="A7:B22" si="1">A6+1</f>
         <v>41399</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C7" s="7">
-        <f t="shared" ref="C7:C25" si="3">E6</f>
-        <v>48</v>
+        <f t="shared" ref="C7:C25" si="2">E6</f>
+        <v>31</v>
       </c>
       <c r="D7" s="7">
         <v>3</v>
       </c>
       <c r="E7" s="40">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2"/>
       <c r="I7" s="41">
-        <f t="shared" si="1"/>
-        <v>48</v>
+        <f t="shared" ref="I7:I26" si="3">I6-TEAM_CAPACITY/$B$26</f>
+        <v>31.64</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
+        <f t="shared" si="1"/>
+        <v>41400</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C8" s="7">
         <f t="shared" si="2"/>
-        <v>41400</v>
-      </c>
-      <c r="B8" s="3">
-        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="D8" s="7">
         <v>3</v>
-      </c>
-      <c r="C8" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0</v>
       </c>
       <c r="E8" s="40">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2"/>
       <c r="I8" s="41">
-        <f t="shared" si="1"/>
-        <v>46</v>
+        <f t="shared" si="3"/>
+        <v>29.96</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
+        <f t="shared" si="1"/>
+        <v>41401</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="7">
         <f t="shared" si="2"/>
-        <v>41401</v>
-      </c>
-      <c r="B9" s="3">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="C9" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D9" s="7">
         <v>0</v>
       </c>
       <c r="E9" s="40">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2"/>
       <c r="I9" s="41">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <f t="shared" si="3"/>
+        <v>28.28</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
+        <f t="shared" si="1"/>
+        <v>41402</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C10" s="7">
         <f t="shared" si="2"/>
-        <v>41402</v>
-      </c>
-      <c r="B10" s="3">
+        <v>25</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4</v>
+      </c>
+      <c r="E10" s="40">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="I10" s="41">
+        <f t="shared" si="3"/>
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <f t="shared" si="1"/>
+        <v>41403</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="40">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="I11" s="41">
+        <f t="shared" si="3"/>
+        <v>24.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <f t="shared" si="1"/>
+        <v>41404</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="40">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="I12" s="41">
+        <f t="shared" si="3"/>
+        <v>23.240000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <f t="shared" si="1"/>
+        <v>41405</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D13" s="7">
+        <v>5</v>
+      </c>
+      <c r="E13" s="40">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="I13" s="41">
+        <f t="shared" si="3"/>
+        <v>21.560000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <f t="shared" si="1"/>
+        <v>41406</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="40">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="I14" s="41">
+        <f t="shared" si="3"/>
+        <v>19.880000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <f t="shared" si="1"/>
+        <v>41407</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D15" s="7">
+        <v>3</v>
+      </c>
+      <c r="E15" s="40">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="I15" s="41">
+        <f t="shared" si="3"/>
+        <v>18.200000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <f t="shared" si="1"/>
+        <v>41408</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="40">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="I16" s="41">
+        <f t="shared" si="3"/>
+        <v>16.520000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f t="shared" si="1"/>
+        <v>41409</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="40">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="I17" s="41">
+        <f t="shared" si="3"/>
+        <v>14.840000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <f t="shared" si="1"/>
+        <v>41410</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="D18" s="7">
+        <v>3</v>
+      </c>
+      <c r="E18" s="40">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="I18" s="41">
+        <f t="shared" si="3"/>
+        <v>13.160000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <f t="shared" si="1"/>
+        <v>41411</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4</v>
+      </c>
+      <c r="E19" s="40">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="I19" s="41">
+        <f t="shared" si="3"/>
+        <v>11.480000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <f t="shared" si="1"/>
+        <v>41412</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0</v>
+      </c>
+      <c r="E20" s="40">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I20" s="41">
+        <f t="shared" si="3"/>
+        <v>9.8000000000000043</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <f t="shared" si="1"/>
+        <v>41413</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="E21" s="40">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I21" s="41">
+        <f>I20-TEAM_CAPACITY/$B$26</f>
+        <v>8.1200000000000045</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <f t="shared" si="1"/>
+        <v>41414</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="C22" s="7">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="C10" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0</v>
-      </c>
-      <c r="E10" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="I10" s="41">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <f t="shared" si="2"/>
-        <v>41403</v>
-      </c>
-      <c r="B11" s="3">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="C11" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="I11" s="41">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <f t="shared" si="2"/>
-        <v>41404</v>
-      </c>
-      <c r="B12" s="3">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="C12" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="I12" s="41">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <f t="shared" si="2"/>
-        <v>41405</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="C13" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="E13" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="I13" s="41">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <f t="shared" si="2"/>
-        <v>41406</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="C14" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="I14" s="41">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <f t="shared" si="2"/>
-        <v>41407</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="C15" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="I15" s="41">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <f t="shared" si="2"/>
-        <v>41408</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="C16" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="I16" s="41">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <f t="shared" si="2"/>
-        <v>41409</v>
-      </c>
-      <c r="B17" s="3">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="C17" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0</v>
-      </c>
-      <c r="E17" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="I17" s="41">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <f t="shared" si="2"/>
-        <v>41410</v>
-      </c>
-      <c r="B18" s="3">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="C18" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D18" s="7">
-        <v>0</v>
-      </c>
-      <c r="E18" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="I18" s="41">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <f t="shared" si="2"/>
-        <v>41411</v>
-      </c>
-      <c r="B19" s="3">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="C19" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D19" s="7">
-        <v>0</v>
-      </c>
-      <c r="E19" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="I19" s="41">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <f t="shared" si="2"/>
-        <v>41412</v>
-      </c>
-      <c r="B20" s="3">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="C20" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="I20" s="41">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <f t="shared" si="2"/>
-        <v>41413</v>
-      </c>
-      <c r="B21" s="3">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="C21" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="I21" s="41">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <f t="shared" si="2"/>
-        <v>41414</v>
-      </c>
-      <c r="B22" s="3">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="C22" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
       <c r="D22" s="7">
         <v>0</v>
       </c>
       <c r="E22" s="40">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F22" s="11"/>
       <c r="I22" s="41">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <f t="shared" si="3"/>
+        <v>6.4400000000000048</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -7489,20 +7495,20 @@
         <v>18</v>
       </c>
       <c r="C23" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="D23" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23" s="40">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F23" s="11"/>
       <c r="I23" s="41">
-        <f t="shared" si="1"/>
-        <v>16</v>
+        <f t="shared" si="3"/>
+        <v>4.7600000000000051</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -7515,20 +7521,20 @@
         <v>19</v>
       </c>
       <c r="C24" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="D24" s="7">
         <v>0</v>
       </c>
       <c r="E24" s="40">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="F24" s="11"/>
       <c r="I24" s="41">
-        <f t="shared" si="1"/>
-        <v>14</v>
+        <f t="shared" si="3"/>
+        <v>3.0800000000000054</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -7541,20 +7547,20 @@
         <v>20</v>
       </c>
       <c r="C25" s="7">
-        <f t="shared" si="3"/>
-        <v>45</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="D25" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E25" s="40">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F25" s="11"/>
       <c r="I25" s="41">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>1.4000000000000055</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -7563,24 +7569,23 @@
         <v>41418</v>
       </c>
       <c r="B26" s="3">
-        <f t="shared" si="4"/>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C26" s="7">
         <f>E25</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="D26" s="7">
         <v>0</v>
       </c>
       <c r="E26" s="40">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F26" s="11"/>
       <c r="I26" s="41">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>-0.27999999999999448</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -7589,11 +7594,11 @@
       </c>
       <c r="B27" s="3">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C27" s="7">
         <f>E26</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="D27" s="7">
         <v>0</v>

</xml_diff>